<commit_message>
updated item transformation diagrams
</commit_message>
<xml_diff>
--- a/item_transformation/diagrams.xlsx
+++ b/item_transformation/diagrams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\DL2020\item_transformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3448B51-51E0-4CF9-8AA0-4E1E89EBE66C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E64924-6AF8-470E-BAAC-CDD684FD8543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCF6DA02-A791-42C3-AA43-031C56B512F7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CCF6DA02-A791-42C3-AA43-031C56B512F7}"/>
   </bookViews>
   <sheets>
     <sheet name="5_epochs" sheetId="2" r:id="rId1"/>
@@ -5666,7 +5666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FA9C04-7449-4DA3-AA7B-41CC6BF6108A}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
@@ -6186,8 +6186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14AAF32-124F-4E67-BE7D-0D938C60366D}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>